<commit_message>
3 fields related to project added in all forms
</commit_message>
<xml_diff>
--- a/app/config/tables/constructionForm/forms/constructionForm/constructionForm.xlsx
+++ b/app/config/tables/constructionForm/forms/constructionForm/constructionForm.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="385">
   <si>
     <t>branch_label</t>
   </si>
@@ -62,6 +62,9 @@
     <t>calculation</t>
   </si>
   <si>
+    <t>display.new_instance_text</t>
+  </si>
+  <si>
     <t>model.isSessionVariable</t>
   </si>
   <si>
@@ -92,9 +95,6 @@
     <t>required</t>
   </si>
   <si>
-    <t>display.new_instance_text</t>
-  </si>
-  <si>
     <t>if // start</t>
   </si>
   <si>
@@ -104,10 +104,34 @@
     <t>Construction Project Details</t>
   </si>
   <si>
+    <t>(opendatakit.getCurrentInstanceId() != null)</t>
+  </si>
+  <si>
     <t>assign</t>
   </si>
   <si>
-    <t>(opendatakit.getCurrentInstanceId() != null)</t>
+    <t>do section survey</t>
+  </si>
+  <si>
+    <t>finalize</t>
+  </si>
+  <si>
+    <t>Save form</t>
+  </si>
+  <si>
+    <t>else // start</t>
+  </si>
+  <si>
+    <t>instances</t>
+  </si>
+  <si>
+    <t>Saved instances</t>
+  </si>
+  <si>
+    <t>end if // start</t>
+  </si>
+  <si>
+    <t>construction_id</t>
   </si>
   <si>
     <t>Notes</t>
@@ -116,51 +140,27 @@
     <t>linked_table</t>
   </si>
   <si>
-    <t>do section survey</t>
-  </si>
-  <si>
-    <t>finalize</t>
-  </si>
-  <si>
     <t>linked_notes</t>
   </si>
   <si>
-    <t>Save form</t>
-  </si>
-  <si>
-    <t>else // start</t>
-  </si>
-  <si>
-    <t>instances</t>
-  </si>
-  <si>
-    <t>Saved instances</t>
-  </si>
-  <si>
-    <t>end if // start</t>
-  </si>
-  <si>
-    <t>construction_id</t>
+    <t>Add Notes to this list</t>
+  </si>
+  <si>
+    <t>Add Note</t>
   </si>
   <si>
     <t>opendatakit.getCurrentInstanceId()</t>
   </si>
   <si>
-    <t>Add Notes to this list</t>
+    <t>end screen</t>
   </si>
   <si>
     <t>string</t>
   </si>
   <si>
-    <t>Add Note</t>
-  </si>
-  <si>
     <t>hidden_input_type.handlebars</t>
   </si>
   <si>
-    <t>end screen</t>
-  </si>
-  <si>
     <t>loc_name</t>
   </si>
   <si>
@@ -236,6 +236,24 @@
     <t>calculates.projectno()</t>
   </si>
   <si>
+    <t>project_correl_id</t>
+  </si>
+  <si>
+    <t>calculates.flowid()</t>
+  </si>
+  <si>
+    <t>project_done</t>
+  </si>
+  <si>
+    <t>calculates.projectdone()</t>
+  </si>
+  <si>
+    <t>project_manager</t>
+  </si>
+  <si>
+    <t>calculates.projectmanager()</t>
+  </si>
+  <si>
     <t>project_comment</t>
   </si>
   <si>
@@ -500,15 +518,6 @@
     <t>calculates.consumableTotalHrs2()</t>
   </si>
   <si>
-    <t>z1_next_photo_index</t>
-  </si>
-  <si>
-    <t>calculates.nextPhotoIndex()</t>
-  </si>
-  <si>
-    <t>integer</t>
-  </si>
-  <si>
     <t>_contents</t>
   </si>
   <si>
@@ -737,12 +746,15 @@
     <t>[ data('construction_id')]</t>
   </si>
   <si>
+    <t>'parent_id='+encodeURIComponent(data('construction_id'))+'&amp;z_pic_name='+encodeURIComponent(data('sample_date').split('/').join('-') + ' - ' + data('loc_name') + ' - ' + opendatakit.total_linked_instances.toString())</t>
+  </si>
+  <si>
+    <t>notesSubform</t>
+  </si>
+  <si>
     <t>'parent_id='+encodeURIComponent(data('construction_id'))</t>
   </si>
   <si>
-    <t>notesSubform</t>
-  </si>
-  <si>
     <t>choice_list_name</t>
   </si>
   <si>
@@ -788,16 +800,22 @@
     <t>Exit.png</t>
   </si>
   <si>
+    <t>yesno</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>calculation_name</t>
-  </si>
-  <si>
-    <t>yesno</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>locationAid</t>
@@ -812,12 +830,6 @@
 })()</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>locationZip</t>
   </si>
   <si>
@@ -842,18 +854,6 @@
 })()</t>
   </si>
   <si>
-    <t>nextPhotoIndex</t>
-  </si>
-  <si>
-    <t>(function(){
-  if (data('z1_next_photo_index')) {
-    return data('z1_next_photo_index');
-  } else {
-    return 0;
-  }
-})()</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
@@ -887,6 +887,42 @@
 })()</t>
   </si>
   <si>
+    <t>flowid</t>
+  </si>
+  <si>
+    <t>(function(){
+  if(opendatakit.getProjectInfo().flowid== ''){
+    return ' ';
+  } else {
+    return opendatakit.getProjectInfo().flowid;
+  }
+})()</t>
+  </si>
+  <si>
+    <t>projectdone</t>
+  </si>
+  <si>
+    <t>(function(){
+  if(opendatakit.getProjectInfo().projectdone== ''){
+    return ' ';
+  } else {
+    return opendatakit.getProjectInfo().projectdone;
+  }
+})()</t>
+  </si>
+  <si>
+    <t>projectmanager</t>
+  </si>
+  <si>
+    <t>(function(){
+  if(opendatakit.getProjectInfo().projectmanager== ''){
+    return ' ';
+  } else {
+    return opendatakit.getProjectInfo().projectmanager;
+  }
+})()</t>
+  </si>
+  <si>
     <t>comment</t>
   </si>
   <si>
@@ -1382,9 +1418,6 @@
     <t>consumableName2</t>
   </si>
   <si>
-    <t>setting_name</t>
-  </si>
-  <si>
     <t>(function(){
   if(opendatakit.getProjectInfo()['consumable_data'] &amp;&amp; opendatakit.getProjectInfo()['consumable_data'][2] &amp;&amp; opendatakit.getProjectInfo()['consumable_data'][2]['selectedconsumable']){
     return opendatakit.getProjectInfo()['consumable_data'][2]['selectedconsumable'];
@@ -1416,6 +1449,9 @@
     return ' ';
   }
 })()</t>
+  </si>
+  <si>
+    <t>setting_name</t>
   </si>
   <si>
     <t>value</t>
@@ -1480,11 +1516,11 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <color rgb="FF444444"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <color rgb="FF444444"/>
       <name val="'Trebuchet MS'"/>
@@ -1517,9 +1553,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1529,28 +1562,37 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -1559,13 +1601,7 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1595,7 +1631,7 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1655,7 +1691,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="29" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="B1" s="29" t="s">
         <v>11</v>
@@ -1663,417 +1699,499 @@
     </row>
     <row r="2">
       <c r="A2" s="29" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="B2" s="39" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="29" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="32" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="32" t="s">
-        <v>266</v>
+      <c r="A5" s="21" t="s">
+        <v>270</v>
       </c>
-      <c r="B5" s="32" t="s">
-        <v>267</v>
+      <c r="B5" s="22" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>268</v>
+        <v>66</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>66</v>
+        <v>273</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="21" t="s">
-        <v>271</v>
+      <c r="A8" s="33" t="s">
+        <v>275</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21"/>
+      <c r="S8" s="21"/>
+      <c r="T8" s="21"/>
+      <c r="U8" s="21"/>
+      <c r="V8" s="21"/>
+      <c r="W8" s="21"/>
+      <c r="X8" s="21"/>
+      <c r="Y8" s="21"/>
+      <c r="Z8" s="21"/>
     </row>
     <row r="9">
-      <c r="A9" s="21" t="s">
-        <v>273</v>
+      <c r="A9" s="33" t="s">
+        <v>277</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="21"/>
+      <c r="T9" s="21"/>
+      <c r="U9" s="21"/>
+      <c r="V9" s="21"/>
+      <c r="W9" s="21"/>
+      <c r="X9" s="21"/>
+      <c r="Y9" s="21"/>
+      <c r="Z9" s="21"/>
     </row>
     <row r="10">
-      <c r="A10" s="21" t="s">
-        <v>275</v>
+      <c r="A10" s="33" t="s">
+        <v>279</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="21"/>
+      <c r="S10" s="21"/>
+      <c r="T10" s="21"/>
+      <c r="U10" s="21"/>
+      <c r="V10" s="21"/>
+      <c r="W10" s="21"/>
+      <c r="X10" s="21"/>
+      <c r="Y10" s="21"/>
+      <c r="Z10" s="21"/>
     </row>
     <row r="11">
-      <c r="A11" s="16" t="s">
-        <v>277</v>
+      <c r="A11" s="21" t="s">
+        <v>281</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="16" t="s">
-        <v>279</v>
+      <c r="A12" s="21" t="s">
+        <v>283</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="16" t="s">
-        <v>281</v>
+      <c r="A13" s="13" t="s">
+        <v>285</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="16" t="s">
-        <v>283</v>
+      <c r="A14" s="13" t="s">
+        <v>287</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="16" t="s">
-        <v>285</v>
+      <c r="A15" s="13" t="s">
+        <v>289</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="16" t="s">
-        <v>287</v>
+      <c r="A16" s="13" t="s">
+        <v>291</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="16" t="s">
-        <v>289</v>
+      <c r="A17" s="13" t="s">
+        <v>293</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="16" t="s">
-        <v>291</v>
+      <c r="A18" s="13" t="s">
+        <v>295</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="16" t="s">
-        <v>293</v>
+      <c r="A19" s="13" t="s">
+        <v>297</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="16" t="s">
-        <v>295</v>
+      <c r="A20" s="13" t="s">
+        <v>299</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="16" t="s">
-        <v>297</v>
+      <c r="A21" s="13" t="s">
+        <v>301</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="16" t="s">
-        <v>299</v>
+      <c r="A22" s="13" t="s">
+        <v>303</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
-        <v>301</v>
+      <c r="A23" s="13" t="s">
+        <v>305</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="16" t="s">
-        <v>303</v>
+      <c r="A24" s="13" t="s">
+        <v>307</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="16" t="s">
-        <v>305</v>
+      <c r="A25" s="13" t="s">
+        <v>309</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="16" t="s">
-        <v>307</v>
+      <c r="A26" s="13" t="s">
+        <v>311</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="16" t="s">
-        <v>309</v>
+      <c r="A27" s="13" t="s">
+        <v>313</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="18" t="s">
-        <v>311</v>
+      <c r="A28" s="13" t="s">
+        <v>315</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="16" t="s">
-        <v>313</v>
+      <c r="A29" s="13" t="s">
+        <v>317</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="16" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="16" t="s">
-        <v>317</v>
+      <c r="A31" s="13" t="s">
+        <v>321</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="16" t="s">
-        <v>319</v>
+      <c r="A32" s="13" t="s">
+        <v>323</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="16" t="s">
-        <v>321</v>
+      <c r="A33" s="13" t="s">
+        <v>325</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="16" t="s">
-        <v>323</v>
+      <c r="A34" s="13" t="s">
+        <v>327</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="16" t="s">
-        <v>325</v>
+      <c r="A35" s="13" t="s">
+        <v>329</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="16" t="s">
-        <v>327</v>
+      <c r="A36" s="13" t="s">
+        <v>331</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="16" t="s">
-        <v>329</v>
+      <c r="A37" s="13" t="s">
+        <v>333</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="16" t="s">
-        <v>331</v>
+      <c r="A38" s="13" t="s">
+        <v>335</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="16" t="s">
-        <v>333</v>
+      <c r="A39" s="13" t="s">
+        <v>337</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="21" t="s">
-        <v>335</v>
+      <c r="A40" s="13" t="s">
+        <v>339</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="21" t="s">
-        <v>337</v>
+      <c r="A41" s="13" t="s">
+        <v>341</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="21" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="21" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="21" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="21" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="B45" s="22" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="21" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="B46" s="22" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="21" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="21" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="21" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="B49" s="22" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="21" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="21" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="B51" s="22" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="21" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="B52" s="22" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="22"/>
+      <c r="A53" s="21" t="s">
+        <v>365</v>
+      </c>
+      <c r="B53" s="22" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="54">
-      <c r="A54" s="21"/>
+      <c r="A54" s="21" t="s">
+        <v>367</v>
+      </c>
+      <c r="B54" s="22" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="22"/>
@@ -2194,6 +2312,12 @@
     </row>
     <row r="94">
       <c r="A94" s="21"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="22"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="21"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2215,13 +2339,13 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="41" t="s">
-        <v>356</v>
+        <v>369</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>362</v>
+        <v>370</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>363</v>
+        <v>371</v>
       </c>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
@@ -2249,10 +2373,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>364</v>
+        <v>372</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>365</v>
+      <c r="B2" s="15" t="s">
+        <v>373</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="7"/>
@@ -2281,9 +2405,9 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>366</v>
+        <v>374</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="15">
         <v>2.0160103E7</v>
       </c>
       <c r="C3" s="1"/>
@@ -2313,11 +2437,11 @@
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>367</v>
+        <v>375</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="11" t="s">
-        <v>368</v>
+      <c r="C4" s="15" t="s">
+        <v>376</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -2344,12 +2468,12 @@
       <c r="Z4" s="7"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="4" t="s">
-        <v>369</v>
+      <c r="A5" s="3" t="s">
+        <v>377</v>
       </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="4" t="s">
-        <v>28</v>
+      <c r="C5" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
@@ -2376,12 +2500,12 @@
       <c r="Z5" s="7"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="4" t="s">
-        <v>370</v>
+      <c r="A6" s="3" t="s">
+        <v>378</v>
       </c>
       <c r="B6" s="1"/>
-      <c r="C6" s="4" t="s">
-        <v>242</v>
+      <c r="C6" s="3" t="s">
+        <v>246</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
@@ -2408,12 +2532,12 @@
       <c r="Z6" s="7"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="4" t="s">
-        <v>371</v>
+      <c r="A7" s="3" t="s">
+        <v>379</v>
       </c>
       <c r="B7" s="1"/>
-      <c r="C7" s="4" t="s">
-        <v>189</v>
+      <c r="C7" s="3" t="s">
+        <v>192</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -2441,11 +2565,11 @@
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="25" t="s">
-        <v>372</v>
+        <v>380</v>
       </c>
       <c r="B8" s="21"/>
       <c r="C8" s="25" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="21"/>
@@ -2473,11 +2597,11 @@
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" s="25" t="s">
-        <v>373</v>
+        <v>381</v>
       </c>
       <c r="B9" s="21"/>
       <c r="C9" s="25" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
@@ -2504,12 +2628,12 @@
       <c r="Z9" s="21"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="4" t="s">
-        <v>374</v>
+      <c r="A10" s="3" t="s">
+        <v>382</v>
       </c>
       <c r="B10" s="1"/>
-      <c r="C10" s="4" t="s">
-        <v>245</v>
+      <c r="C10" s="3" t="s">
+        <v>249</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
@@ -2536,12 +2660,12 @@
       <c r="Z10" s="7"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="4" t="s">
-        <v>375</v>
+      <c r="A11" s="3" t="s">
+        <v>383</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="4" t="s">
-        <v>247</v>
+      <c r="C11" s="3" t="s">
+        <v>251</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -2568,12 +2692,12 @@
       <c r="Z11" s="7"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="4" t="s">
-        <v>376</v>
+      <c r="A12" s="3" t="s">
+        <v>384</v>
       </c>
       <c r="B12" s="1"/>
-      <c r="C12" s="4" t="s">
-        <v>250</v>
+      <c r="C12" s="3" t="s">
+        <v>254</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>

</xml_diff>